<commit_message>
update source for hosting OA
</commit_message>
<xml_diff>
--- a/tmpA3.xlsx
+++ b/tmpA3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DaiLamMoc\KeToanDaiLamMoc\DaiLamMoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236286CE-D7F1-4D10-A770-212B7CB1D944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D34EB8-99FB-4934-A8FA-E5DCA6AF35E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="2430" windowWidth="19545" windowHeight="13770" xr2:uid="{7295F9C0-1D23-42CE-9F19-08E01B072D9F}"/>
   </bookViews>
@@ -722,7 +722,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -924,6 +924,72 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="16" fillId="4" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="4" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="4" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="4" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="4" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="13" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -945,70 +1011,22 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="16" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="4" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="4" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="4" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="4" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="4" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1434,11 +1452,11 @@
   <dimension ref="A1:Z152"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
       <selection activeCell="Q19" sqref="Q19:Q21"/>
       <selection pane="topRight" activeCell="Q19" sqref="Q19:Q21"/>
       <selection pane="bottomLeft" activeCell="Q19" sqref="Q19:Q21"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14:Q135"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="25.5" customHeight="1"/>
@@ -1452,7 +1470,7 @@
     <col min="7" max="7" width="11.85546875" style="6" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" style="6" customWidth="1"/>
     <col min="9" max="9" width="7.7109375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14" style="71" customWidth="1"/>
+    <col min="10" max="10" width="14" style="107" customWidth="1"/>
     <col min="11" max="11" width="7.140625" style="6" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="6" customWidth="1"/>
     <col min="13" max="13" width="11" style="6" customWidth="1"/>
@@ -1484,231 +1502,231 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="4"/>
+      <c r="J1" s="102"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="4"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
-      <c r="W1" s="74"/>
-      <c r="X1" s="74"/>
-      <c r="Y1" s="74"/>
-      <c r="Z1" s="74"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
+      <c r="T1" s="96"/>
+      <c r="U1" s="96"/>
+      <c r="V1" s="96"/>
+      <c r="W1" s="96"/>
+      <c r="X1" s="96"/>
+      <c r="Y1" s="96"/>
+      <c r="Z1" s="96"/>
     </row>
     <row r="2" spans="1:26" ht="25.5" customHeight="1">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
       <c r="P2" s="7"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="75"/>
-      <c r="Z2" s="75"/>
+      <c r="Q2" s="97"/>
+      <c r="R2" s="97"/>
+      <c r="S2" s="97"/>
+      <c r="T2" s="97"/>
+      <c r="U2" s="97"/>
+      <c r="V2" s="97"/>
+      <c r="W2" s="97"/>
+      <c r="X2" s="97"/>
+      <c r="Y2" s="97"/>
+      <c r="Z2" s="97"/>
     </row>
     <row r="3" spans="1:26" ht="25.5" customHeight="1">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
       <c r="P3" s="7"/>
-      <c r="Q3" s="75"/>
-      <c r="R3" s="75"/>
-      <c r="S3" s="75"/>
-      <c r="T3" s="75"/>
-      <c r="U3" s="75"/>
-      <c r="V3" s="75"/>
-      <c r="W3" s="75"/>
-      <c r="X3" s="75"/>
-      <c r="Y3" s="75"/>
-      <c r="Z3" s="75"/>
+      <c r="Q3" s="97"/>
+      <c r="R3" s="97"/>
+      <c r="S3" s="97"/>
+      <c r="T3" s="97"/>
+      <c r="U3" s="97"/>
+      <c r="V3" s="97"/>
+      <c r="W3" s="97"/>
+      <c r="X3" s="97"/>
+      <c r="Y3" s="97"/>
+      <c r="Z3" s="97"/>
     </row>
     <row r="4" spans="1:26" ht="25.5" customHeight="1">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
+      <c r="B4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
       <c r="P4" s="7"/>
-      <c r="Q4" s="75"/>
-      <c r="R4" s="75"/>
-      <c r="S4" s="75"/>
-      <c r="T4" s="75"/>
-      <c r="U4" s="75"/>
-      <c r="V4" s="75"/>
-      <c r="W4" s="75"/>
-      <c r="X4" s="75"/>
-      <c r="Y4" s="75"/>
-      <c r="Z4" s="75"/>
+      <c r="Q4" s="97"/>
+      <c r="R4" s="97"/>
+      <c r="S4" s="97"/>
+      <c r="T4" s="97"/>
+      <c r="U4" s="97"/>
+      <c r="V4" s="97"/>
+      <c r="W4" s="97"/>
+      <c r="X4" s="97"/>
+      <c r="Y4" s="97"/>
+      <c r="Z4" s="97"/>
     </row>
     <row r="5" spans="1:26" ht="25.5" customHeight="1">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="97"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="11"/>
-      <c r="Q5" s="75"/>
-      <c r="R5" s="75"/>
-      <c r="S5" s="75"/>
-      <c r="T5" s="75"/>
-      <c r="U5" s="75"/>
-      <c r="V5" s="75"/>
-      <c r="W5" s="75"/>
-      <c r="X5" s="75"/>
-      <c r="Y5" s="75"/>
-      <c r="Z5" s="75"/>
+      <c r="Q5" s="97"/>
+      <c r="R5" s="97"/>
+      <c r="S5" s="97"/>
+      <c r="T5" s="97"/>
+      <c r="U5" s="97"/>
+      <c r="V5" s="97"/>
+      <c r="W5" s="97"/>
+      <c r="X5" s="97"/>
+      <c r="Y5" s="97"/>
+      <c r="Z5" s="97"/>
     </row>
     <row r="6" spans="1:26" ht="25.5" customHeight="1">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="77"/>
-      <c r="O6" s="77"/>
-      <c r="P6" s="77"/>
-      <c r="Q6" s="77"/>
-      <c r="R6" s="77"/>
-      <c r="S6" s="77"/>
-      <c r="T6" s="77"/>
-      <c r="U6" s="77"/>
-      <c r="V6" s="77"/>
-      <c r="W6" s="77"/>
-      <c r="X6" s="77"/>
-      <c r="Y6" s="77"/>
-      <c r="Z6" s="77"/>
+      <c r="B6" s="99"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="99"/>
+      <c r="N6" s="99"/>
+      <c r="O6" s="99"/>
+      <c r="P6" s="99"/>
+      <c r="Q6" s="99"/>
+      <c r="R6" s="99"/>
+      <c r="S6" s="99"/>
+      <c r="T6" s="99"/>
+      <c r="U6" s="99"/>
+      <c r="V6" s="99"/>
+      <c r="W6" s="99"/>
+      <c r="X6" s="99"/>
+      <c r="Y6" s="99"/>
+      <c r="Z6" s="99"/>
     </row>
     <row r="7" spans="1:26" ht="25.5" customHeight="1">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="78"/>
-      <c r="M7" s="78"/>
-      <c r="N7" s="78"/>
-      <c r="O7" s="78"/>
-      <c r="P7" s="78"/>
-      <c r="Q7" s="78"/>
-      <c r="R7" s="78"/>
-      <c r="S7" s="78"/>
-      <c r="T7" s="78"/>
-      <c r="U7" s="78"/>
-      <c r="V7" s="78"/>
-      <c r="W7" s="78"/>
-      <c r="X7" s="78"/>
-      <c r="Y7" s="78"/>
-      <c r="Z7" s="78"/>
+      <c r="B7" s="100"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="100"/>
+      <c r="J7" s="100"/>
+      <c r="K7" s="100"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
+      <c r="N7" s="100"/>
+      <c r="O7" s="100"/>
+      <c r="P7" s="100"/>
+      <c r="Q7" s="100"/>
+      <c r="R7" s="100"/>
+      <c r="S7" s="100"/>
+      <c r="T7" s="100"/>
+      <c r="U7" s="100"/>
+      <c r="V7" s="100"/>
+      <c r="W7" s="100"/>
+      <c r="X7" s="100"/>
+      <c r="Y7" s="100"/>
+      <c r="Z7" s="100"/>
     </row>
     <row r="8" spans="1:26" ht="25.5" customHeight="1">
       <c r="A8" s="12"/>
       <c r="B8" s="13"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
-      <c r="I8" s="79"/>
-      <c r="J8" s="79"/>
-      <c r="K8" s="79"/>
-      <c r="L8" s="79"/>
-      <c r="M8" s="79"/>
-      <c r="N8" s="79"/>
-      <c r="O8" s="79"/>
-      <c r="P8" s="79"/>
-      <c r="Q8" s="79"/>
-      <c r="R8" s="79"/>
-      <c r="S8" s="79"/>
-      <c r="T8" s="79"/>
-      <c r="U8" s="79"/>
-      <c r="V8" s="79"/>
-      <c r="W8" s="79"/>
-      <c r="X8" s="79"/>
-      <c r="Y8" s="79"/>
-      <c r="Z8" s="79"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="101"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="101"/>
+      <c r="M8" s="101"/>
+      <c r="N8" s="101"/>
+      <c r="O8" s="101"/>
+      <c r="P8" s="101"/>
+      <c r="Q8" s="101"/>
+      <c r="R8" s="101"/>
+      <c r="S8" s="101"/>
+      <c r="T8" s="101"/>
+      <c r="U8" s="101"/>
+      <c r="V8" s="101"/>
+      <c r="W8" s="101"/>
+      <c r="X8" s="101"/>
+      <c r="Y8" s="101"/>
+      <c r="Z8" s="101"/>
     </row>
     <row r="9" spans="1:26" ht="25.5" customHeight="1">
       <c r="A9" s="14"/>
@@ -1717,15 +1735,15 @@
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="73">
+      <c r="E9" s="95">
         <f>+'[1]25.9'!E17:F17</f>
         <v>1899002428.4285715</v>
       </c>
-      <c r="F9" s="73"/>
+      <c r="F9" s="95"/>
       <c r="G9" s="18"/>
       <c r="H9" s="19"/>
       <c r="I9" s="20"/>
-      <c r="J9" s="21"/>
+      <c r="J9" s="104"/>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
@@ -1750,15 +1768,15 @@
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="24"/>
-      <c r="E10" s="80">
+      <c r="E10" s="91">
         <f>+Y150</f>
         <v>0</v>
       </c>
-      <c r="F10" s="80"/>
+      <c r="F10" s="91"/>
       <c r="G10" s="25"/>
       <c r="H10" s="26"/>
       <c r="I10" s="20"/>
-      <c r="J10" s="21"/>
+      <c r="J10" s="104"/>
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
@@ -1786,7 +1804,7 @@
       <c r="G11" s="28"/>
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
-      <c r="J11" s="28"/>
+      <c r="J11" s="29"/>
       <c r="K11" s="29"/>
       <c r="L11" s="29"/>
       <c r="M11" s="29"/>
@@ -1807,114 +1825,114 @@
       </c>
     </row>
     <row r="12" spans="1:26" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="83" t="s">
+      <c r="C12" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="85"/>
-      <c r="E12" s="83" t="s">
+      <c r="D12" s="94"/>
+      <c r="E12" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="83" t="s">
+      <c r="F12" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="88" t="s">
+      <c r="G12" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="90" t="s">
+      <c r="H12" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="83" t="s">
+      <c r="I12" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="83" t="s">
+      <c r="J12" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="83" t="s">
+      <c r="K12" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="83" t="s">
+      <c r="L12" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="M12" s="83" t="s">
+      <c r="M12" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="N12" s="98" t="s">
+      <c r="N12" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="O12" s="98" t="s">
+      <c r="O12" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="P12" s="83" t="s">
+      <c r="P12" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="Q12" s="100" t="s">
+      <c r="Q12" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="R12" s="86" t="s">
+      <c r="R12" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="S12" s="86" t="s">
+      <c r="S12" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="T12" s="96" t="s">
+      <c r="T12" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="U12" s="86" t="s">
+      <c r="U12" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="V12" s="86" t="s">
+      <c r="V12" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="W12" s="86" t="s">
+      <c r="W12" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="X12" s="96" t="s">
+      <c r="X12" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="Y12" s="86" t="s">
+      <c r="Y12" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="Z12" s="92" t="s">
+      <c r="Z12" s="75" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:26" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A13" s="82"/>
-      <c r="B13" s="84"/>
+      <c r="A13" s="93"/>
+      <c r="B13" s="82"/>
       <c r="C13" s="33" t="s">
         <v>34</v>
       </c>
       <c r="D13" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="84"/>
-      <c r="F13" s="84"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="91"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="88"/>
-      <c r="L13" s="88"/>
-      <c r="M13" s="84"/>
-      <c r="N13" s="99"/>
-      <c r="O13" s="99"/>
-      <c r="P13" s="88"/>
-      <c r="Q13" s="101"/>
-      <c r="R13" s="87"/>
-      <c r="S13" s="87"/>
-      <c r="T13" s="97"/>
-      <c r="U13" s="87"/>
-      <c r="V13" s="87"/>
-      <c r="W13" s="87"/>
-      <c r="X13" s="97"/>
-      <c r="Y13" s="87"/>
-      <c r="Z13" s="93"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="103"/>
+      <c r="K13" s="85"/>
+      <c r="L13" s="85"/>
+      <c r="M13" s="82"/>
+      <c r="N13" s="84"/>
+      <c r="O13" s="84"/>
+      <c r="P13" s="85"/>
+      <c r="Q13" s="87"/>
+      <c r="R13" s="74"/>
+      <c r="S13" s="74"/>
+      <c r="T13" s="80"/>
+      <c r="U13" s="74"/>
+      <c r="V13" s="74"/>
+      <c r="W13" s="74"/>
+      <c r="X13" s="80"/>
+      <c r="Y13" s="74"/>
+      <c r="Z13" s="76"/>
     </row>
     <row r="14" spans="1:26" s="34" customFormat="1" ht="52.5" customHeight="1">
       <c r="A14" s="48"/>
@@ -1926,7 +1944,7 @@
       <c r="G14" s="36"/>
       <c r="H14" s="37"/>
       <c r="I14" s="36"/>
-      <c r="J14" s="47"/>
+      <c r="J14" s="43"/>
       <c r="K14" s="36"/>
       <c r="L14" s="36"/>
       <c r="M14" s="37"/>
@@ -1957,7 +1975,7 @@
       <c r="G15" s="36"/>
       <c r="H15" s="37"/>
       <c r="I15" s="36"/>
-      <c r="J15" s="47"/>
+      <c r="J15" s="43"/>
       <c r="K15" s="36"/>
       <c r="L15" s="36"/>
       <c r="M15" s="37"/>
@@ -1988,7 +2006,7 @@
       <c r="G16" s="36"/>
       <c r="H16" s="37"/>
       <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
+      <c r="J16" s="43"/>
       <c r="K16" s="36"/>
       <c r="L16" s="36"/>
       <c r="M16" s="37"/>
@@ -2019,7 +2037,7 @@
       <c r="G17" s="36"/>
       <c r="H17" s="37"/>
       <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
+      <c r="J17" s="43"/>
       <c r="K17" s="36"/>
       <c r="L17" s="36"/>
       <c r="M17" s="37"/>
@@ -2050,7 +2068,7 @@
       <c r="G18" s="44"/>
       <c r="H18" s="37"/>
       <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
+      <c r="J18" s="43"/>
       <c r="K18" s="36"/>
       <c r="L18" s="36"/>
       <c r="M18" s="37"/>
@@ -2081,7 +2099,7 @@
       <c r="G19" s="44"/>
       <c r="H19" s="37"/>
       <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
+      <c r="J19" s="43"/>
       <c r="K19" s="36"/>
       <c r="L19" s="36"/>
       <c r="M19" s="37"/>
@@ -2112,7 +2130,7 @@
       <c r="G20" s="44"/>
       <c r="H20" s="37"/>
       <c r="I20" s="36"/>
-      <c r="J20" s="47"/>
+      <c r="J20" s="43"/>
       <c r="K20" s="36"/>
       <c r="L20" s="36"/>
       <c r="M20" s="37"/>
@@ -2143,7 +2161,7 @@
       <c r="G21" s="36"/>
       <c r="H21" s="37"/>
       <c r="I21" s="36"/>
-      <c r="J21" s="47"/>
+      <c r="J21" s="43"/>
       <c r="K21" s="36"/>
       <c r="L21" s="36"/>
       <c r="M21" s="37"/>
@@ -2174,7 +2192,7 @@
       <c r="G22" s="36"/>
       <c r="H22" s="37"/>
       <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
+      <c r="J22" s="43"/>
       <c r="K22" s="36"/>
       <c r="L22" s="36"/>
       <c r="M22" s="37"/>
@@ -2205,7 +2223,7 @@
       <c r="G23" s="36"/>
       <c r="H23" s="37"/>
       <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
+      <c r="J23" s="43"/>
       <c r="K23" s="36"/>
       <c r="L23" s="36"/>
       <c r="M23" s="37"/>
@@ -2236,7 +2254,7 @@
       <c r="G24" s="36"/>
       <c r="H24" s="37"/>
       <c r="I24" s="36"/>
-      <c r="J24" s="47"/>
+      <c r="J24" s="43"/>
       <c r="K24" s="36"/>
       <c r="L24" s="36"/>
       <c r="M24" s="37"/>
@@ -2267,7 +2285,7 @@
       <c r="G25" s="36"/>
       <c r="H25" s="37"/>
       <c r="I25" s="36"/>
-      <c r="J25" s="47"/>
+      <c r="J25" s="43"/>
       <c r="K25" s="36"/>
       <c r="L25" s="36"/>
       <c r="M25" s="37"/>
@@ -2298,7 +2316,7 @@
       <c r="G26" s="36"/>
       <c r="H26" s="37"/>
       <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
+      <c r="J26" s="43"/>
       <c r="K26" s="36"/>
       <c r="L26" s="36"/>
       <c r="M26" s="37"/>
@@ -2329,7 +2347,7 @@
       <c r="G27" s="36"/>
       <c r="H27" s="37"/>
       <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="J27" s="43"/>
       <c r="K27" s="36"/>
       <c r="L27" s="36"/>
       <c r="M27" s="37"/>
@@ -2360,7 +2378,7 @@
       <c r="G28" s="36"/>
       <c r="H28" s="37"/>
       <c r="I28" s="36"/>
-      <c r="J28" s="47"/>
+      <c r="J28" s="43"/>
       <c r="K28" s="36"/>
       <c r="L28" s="36"/>
       <c r="M28" s="37"/>
@@ -2391,7 +2409,7 @@
       <c r="G29" s="36"/>
       <c r="H29" s="37"/>
       <c r="I29" s="36"/>
-      <c r="J29" s="47"/>
+      <c r="J29" s="43"/>
       <c r="K29" s="36"/>
       <c r="L29" s="36"/>
       <c r="M29" s="37"/>
@@ -2422,7 +2440,7 @@
       <c r="G30" s="36"/>
       <c r="H30" s="37"/>
       <c r="I30" s="36"/>
-      <c r="J30" s="36"/>
+      <c r="J30" s="43"/>
       <c r="K30" s="36"/>
       <c r="L30" s="36"/>
       <c r="M30" s="37"/>
@@ -2453,7 +2471,7 @@
       <c r="G31" s="36"/>
       <c r="H31" s="37"/>
       <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
+      <c r="J31" s="43"/>
       <c r="K31" s="36"/>
       <c r="L31" s="36"/>
       <c r="M31" s="37"/>
@@ -2484,7 +2502,7 @@
       <c r="G32" s="44"/>
       <c r="H32" s="37"/>
       <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
+      <c r="J32" s="43"/>
       <c r="K32" s="36"/>
       <c r="L32" s="36"/>
       <c r="M32" s="37"/>
@@ -2515,7 +2533,7 @@
       <c r="G33" s="44"/>
       <c r="H33" s="37"/>
       <c r="I33" s="36"/>
-      <c r="J33" s="36"/>
+      <c r="J33" s="43"/>
       <c r="K33" s="36"/>
       <c r="L33" s="36"/>
       <c r="M33" s="37"/>
@@ -2546,7 +2564,7 @@
       <c r="G34" s="44"/>
       <c r="H34" s="37"/>
       <c r="I34" s="36"/>
-      <c r="J34" s="47"/>
+      <c r="J34" s="43"/>
       <c r="K34" s="36"/>
       <c r="L34" s="36"/>
       <c r="M34" s="37"/>
@@ -2577,7 +2595,7 @@
       <c r="G35" s="36"/>
       <c r="H35" s="37"/>
       <c r="I35" s="36"/>
-      <c r="J35" s="47"/>
+      <c r="J35" s="43"/>
       <c r="K35" s="36"/>
       <c r="L35" s="36"/>
       <c r="M35" s="37"/>
@@ -2608,7 +2626,7 @@
       <c r="G36" s="36"/>
       <c r="H36" s="37"/>
       <c r="I36" s="36"/>
-      <c r="J36" s="36"/>
+      <c r="J36" s="43"/>
       <c r="K36" s="36"/>
       <c r="L36" s="36"/>
       <c r="M36" s="37"/>
@@ -2639,7 +2657,7 @@
       <c r="G37" s="36"/>
       <c r="H37" s="37"/>
       <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="J37" s="43"/>
       <c r="K37" s="36"/>
       <c r="L37" s="36"/>
       <c r="M37" s="37"/>
@@ -2670,7 +2688,7 @@
       <c r="G38" s="36"/>
       <c r="H38" s="37"/>
       <c r="I38" s="36"/>
-      <c r="J38" s="47"/>
+      <c r="J38" s="43"/>
       <c r="K38" s="36"/>
       <c r="L38" s="36"/>
       <c r="M38" s="37"/>
@@ -2701,7 +2719,7 @@
       <c r="G39" s="36"/>
       <c r="H39" s="37"/>
       <c r="I39" s="36"/>
-      <c r="J39" s="47"/>
+      <c r="J39" s="43"/>
       <c r="K39" s="36"/>
       <c r="L39" s="36"/>
       <c r="M39" s="37"/>
@@ -2732,7 +2750,7 @@
       <c r="G40" s="36"/>
       <c r="H40" s="37"/>
       <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
+      <c r="J40" s="43"/>
       <c r="K40" s="36"/>
       <c r="L40" s="36"/>
       <c r="M40" s="37"/>
@@ -2763,7 +2781,7 @@
       <c r="G41" s="36"/>
       <c r="H41" s="37"/>
       <c r="I41" s="36"/>
-      <c r="J41" s="36"/>
+      <c r="J41" s="43"/>
       <c r="K41" s="36"/>
       <c r="L41" s="36"/>
       <c r="M41" s="37"/>
@@ -2794,7 +2812,7 @@
       <c r="G42" s="36"/>
       <c r="H42" s="37"/>
       <c r="I42" s="36"/>
-      <c r="J42" s="47"/>
+      <c r="J42" s="43"/>
       <c r="K42" s="36"/>
       <c r="L42" s="36"/>
       <c r="M42" s="37"/>
@@ -2825,7 +2843,7 @@
       <c r="G43" s="36"/>
       <c r="H43" s="37"/>
       <c r="I43" s="36"/>
-      <c r="J43" s="47"/>
+      <c r="J43" s="43"/>
       <c r="K43" s="36"/>
       <c r="L43" s="36"/>
       <c r="M43" s="37"/>
@@ -2856,7 +2874,7 @@
       <c r="G44" s="36"/>
       <c r="H44" s="37"/>
       <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="J44" s="43"/>
       <c r="K44" s="36"/>
       <c r="L44" s="36"/>
       <c r="M44" s="37"/>
@@ -2887,7 +2905,7 @@
       <c r="G45" s="36"/>
       <c r="H45" s="37"/>
       <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="J45" s="43"/>
       <c r="K45" s="36"/>
       <c r="L45" s="36"/>
       <c r="M45" s="37"/>
@@ -2918,7 +2936,7 @@
       <c r="G46" s="44"/>
       <c r="H46" s="37"/>
       <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="J46" s="43"/>
       <c r="K46" s="36"/>
       <c r="L46" s="36"/>
       <c r="M46" s="37"/>
@@ -2949,7 +2967,7 @@
       <c r="G47" s="44"/>
       <c r="H47" s="37"/>
       <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="J47" s="43"/>
       <c r="K47" s="36"/>
       <c r="L47" s="36"/>
       <c r="M47" s="37"/>
@@ -2980,7 +2998,7 @@
       <c r="G48" s="44"/>
       <c r="H48" s="37"/>
       <c r="I48" s="36"/>
-      <c r="J48" s="47"/>
+      <c r="J48" s="43"/>
       <c r="K48" s="36"/>
       <c r="L48" s="36"/>
       <c r="M48" s="37"/>
@@ -3011,7 +3029,7 @@
       <c r="G49" s="36"/>
       <c r="H49" s="37"/>
       <c r="I49" s="36"/>
-      <c r="J49" s="47"/>
+      <c r="J49" s="43"/>
       <c r="K49" s="36"/>
       <c r="L49" s="36"/>
       <c r="M49" s="37"/>
@@ -3042,7 +3060,7 @@
       <c r="G50" s="36"/>
       <c r="H50" s="37"/>
       <c r="I50" s="36"/>
-      <c r="J50" s="36"/>
+      <c r="J50" s="43"/>
       <c r="K50" s="36"/>
       <c r="L50" s="36"/>
       <c r="M50" s="37"/>
@@ -3073,7 +3091,7 @@
       <c r="G51" s="36"/>
       <c r="H51" s="37"/>
       <c r="I51" s="36"/>
-      <c r="J51" s="36"/>
+      <c r="J51" s="43"/>
       <c r="K51" s="36"/>
       <c r="L51" s="36"/>
       <c r="M51" s="37"/>
@@ -3104,7 +3122,7 @@
       <c r="G52" s="36"/>
       <c r="H52" s="37"/>
       <c r="I52" s="36"/>
-      <c r="J52" s="47"/>
+      <c r="J52" s="43"/>
       <c r="K52" s="36"/>
       <c r="L52" s="36"/>
       <c r="M52" s="37"/>
@@ -3135,7 +3153,7 @@
       <c r="G53" s="36"/>
       <c r="H53" s="37"/>
       <c r="I53" s="36"/>
-      <c r="J53" s="47"/>
+      <c r="J53" s="43"/>
       <c r="K53" s="36"/>
       <c r="L53" s="36"/>
       <c r="M53" s="37"/>
@@ -3166,7 +3184,7 @@
       <c r="G54" s="36"/>
       <c r="H54" s="37"/>
       <c r="I54" s="36"/>
-      <c r="J54" s="36"/>
+      <c r="J54" s="43"/>
       <c r="K54" s="36"/>
       <c r="L54" s="36"/>
       <c r="M54" s="37"/>
@@ -3197,7 +3215,7 @@
       <c r="G55" s="36"/>
       <c r="H55" s="37"/>
       <c r="I55" s="36"/>
-      <c r="J55" s="36"/>
+      <c r="J55" s="43"/>
       <c r="K55" s="36"/>
       <c r="L55" s="36"/>
       <c r="M55" s="37"/>
@@ -3228,7 +3246,7 @@
       <c r="G56" s="36"/>
       <c r="H56" s="37"/>
       <c r="I56" s="36"/>
-      <c r="J56" s="47"/>
+      <c r="J56" s="43"/>
       <c r="K56" s="36"/>
       <c r="L56" s="36"/>
       <c r="M56" s="37"/>
@@ -3259,7 +3277,7 @@
       <c r="G57" s="36"/>
       <c r="H57" s="37"/>
       <c r="I57" s="36"/>
-      <c r="J57" s="47"/>
+      <c r="J57" s="43"/>
       <c r="K57" s="36"/>
       <c r="L57" s="36"/>
       <c r="M57" s="37"/>
@@ -3290,7 +3308,7 @@
       <c r="G58" s="36"/>
       <c r="H58" s="37"/>
       <c r="I58" s="36"/>
-      <c r="J58" s="36"/>
+      <c r="J58" s="43"/>
       <c r="K58" s="36"/>
       <c r="L58" s="36"/>
       <c r="M58" s="37"/>
@@ -3321,7 +3339,7 @@
       <c r="G59" s="36"/>
       <c r="H59" s="37"/>
       <c r="I59" s="36"/>
-      <c r="J59" s="36"/>
+      <c r="J59" s="43"/>
       <c r="K59" s="36"/>
       <c r="L59" s="36"/>
       <c r="M59" s="37"/>
@@ -3352,7 +3370,7 @@
       <c r="G60" s="44"/>
       <c r="H60" s="37"/>
       <c r="I60" s="36"/>
-      <c r="J60" s="36"/>
+      <c r="J60" s="43"/>
       <c r="K60" s="36"/>
       <c r="L60" s="36"/>
       <c r="M60" s="37"/>
@@ -3383,7 +3401,7 @@
       <c r="G61" s="44"/>
       <c r="H61" s="37"/>
       <c r="I61" s="36"/>
-      <c r="J61" s="36"/>
+      <c r="J61" s="43"/>
       <c r="K61" s="36"/>
       <c r="L61" s="36"/>
       <c r="M61" s="37"/>
@@ -3414,7 +3432,7 @@
       <c r="G62" s="44"/>
       <c r="H62" s="37"/>
       <c r="I62" s="36"/>
-      <c r="J62" s="47"/>
+      <c r="J62" s="43"/>
       <c r="K62" s="36"/>
       <c r="L62" s="36"/>
       <c r="M62" s="37"/>
@@ -3445,7 +3463,7 @@
       <c r="G63" s="36"/>
       <c r="H63" s="37"/>
       <c r="I63" s="36"/>
-      <c r="J63" s="47"/>
+      <c r="J63" s="43"/>
       <c r="K63" s="36"/>
       <c r="L63" s="36"/>
       <c r="M63" s="37"/>
@@ -3476,7 +3494,7 @@
       <c r="G64" s="36"/>
       <c r="H64" s="37"/>
       <c r="I64" s="36"/>
-      <c r="J64" s="36"/>
+      <c r="J64" s="43"/>
       <c r="K64" s="36"/>
       <c r="L64" s="36"/>
       <c r="M64" s="37"/>
@@ -3507,7 +3525,7 @@
       <c r="G65" s="36"/>
       <c r="H65" s="37"/>
       <c r="I65" s="36"/>
-      <c r="J65" s="36"/>
+      <c r="J65" s="43"/>
       <c r="K65" s="36"/>
       <c r="L65" s="36"/>
       <c r="M65" s="37"/>
@@ -3538,7 +3556,7 @@
       <c r="G66" s="36"/>
       <c r="H66" s="37"/>
       <c r="I66" s="36"/>
-      <c r="J66" s="47"/>
+      <c r="J66" s="43"/>
       <c r="K66" s="36"/>
       <c r="L66" s="36"/>
       <c r="M66" s="37"/>
@@ -3569,7 +3587,7 @@
       <c r="G67" s="36"/>
       <c r="H67" s="37"/>
       <c r="I67" s="36"/>
-      <c r="J67" s="47"/>
+      <c r="J67" s="43"/>
       <c r="K67" s="36"/>
       <c r="L67" s="36"/>
       <c r="M67" s="37"/>
@@ -3600,7 +3618,7 @@
       <c r="G68" s="36"/>
       <c r="H68" s="37"/>
       <c r="I68" s="36"/>
-      <c r="J68" s="36"/>
+      <c r="J68" s="43"/>
       <c r="K68" s="36"/>
       <c r="L68" s="36"/>
       <c r="M68" s="37"/>
@@ -3631,7 +3649,7 @@
       <c r="G69" s="36"/>
       <c r="H69" s="37"/>
       <c r="I69" s="36"/>
-      <c r="J69" s="36"/>
+      <c r="J69" s="43"/>
       <c r="K69" s="36"/>
       <c r="L69" s="36"/>
       <c r="M69" s="37"/>
@@ -3662,7 +3680,7 @@
       <c r="G70" s="36"/>
       <c r="H70" s="37"/>
       <c r="I70" s="36"/>
-      <c r="J70" s="47"/>
+      <c r="J70" s="43"/>
       <c r="K70" s="36"/>
       <c r="L70" s="36"/>
       <c r="M70" s="37"/>
@@ -3693,7 +3711,7 @@
       <c r="G71" s="36"/>
       <c r="H71" s="37"/>
       <c r="I71" s="36"/>
-      <c r="J71" s="47"/>
+      <c r="J71" s="43"/>
       <c r="K71" s="36"/>
       <c r="L71" s="36"/>
       <c r="M71" s="37"/>
@@ -3724,7 +3742,7 @@
       <c r="G72" s="36"/>
       <c r="H72" s="37"/>
       <c r="I72" s="36"/>
-      <c r="J72" s="36"/>
+      <c r="J72" s="43"/>
       <c r="K72" s="36"/>
       <c r="L72" s="36"/>
       <c r="M72" s="37"/>
@@ -3755,7 +3773,7 @@
       <c r="G73" s="36"/>
       <c r="H73" s="37"/>
       <c r="I73" s="36"/>
-      <c r="J73" s="36"/>
+      <c r="J73" s="43"/>
       <c r="K73" s="36"/>
       <c r="L73" s="36"/>
       <c r="M73" s="37"/>
@@ -3786,7 +3804,7 @@
       <c r="G74" s="44"/>
       <c r="H74" s="37"/>
       <c r="I74" s="36"/>
-      <c r="J74" s="36"/>
+      <c r="J74" s="43"/>
       <c r="K74" s="36"/>
       <c r="L74" s="36"/>
       <c r="M74" s="37"/>
@@ -3817,7 +3835,7 @@
       <c r="G75" s="44"/>
       <c r="H75" s="37"/>
       <c r="I75" s="36"/>
-      <c r="J75" s="36"/>
+      <c r="J75" s="43"/>
       <c r="K75" s="36"/>
       <c r="L75" s="36"/>
       <c r="M75" s="37"/>
@@ -3848,7 +3866,7 @@
       <c r="G76" s="44"/>
       <c r="H76" s="37"/>
       <c r="I76" s="36"/>
-      <c r="J76" s="47"/>
+      <c r="J76" s="43"/>
       <c r="K76" s="36"/>
       <c r="L76" s="36"/>
       <c r="M76" s="37"/>
@@ -3879,7 +3897,7 @@
       <c r="G77" s="36"/>
       <c r="H77" s="37"/>
       <c r="I77" s="36"/>
-      <c r="J77" s="47"/>
+      <c r="J77" s="43"/>
       <c r="K77" s="36"/>
       <c r="L77" s="36"/>
       <c r="M77" s="37"/>
@@ -3910,7 +3928,7 @@
       <c r="G78" s="36"/>
       <c r="H78" s="37"/>
       <c r="I78" s="36"/>
-      <c r="J78" s="36"/>
+      <c r="J78" s="43"/>
       <c r="K78" s="36"/>
       <c r="L78" s="36"/>
       <c r="M78" s="37"/>
@@ -3941,7 +3959,7 @@
       <c r="G79" s="36"/>
       <c r="H79" s="37"/>
       <c r="I79" s="36"/>
-      <c r="J79" s="36"/>
+      <c r="J79" s="43"/>
       <c r="K79" s="36"/>
       <c r="L79" s="36"/>
       <c r="M79" s="37"/>
@@ -3972,7 +3990,7 @@
       <c r="G80" s="36"/>
       <c r="H80" s="37"/>
       <c r="I80" s="36"/>
-      <c r="J80" s="47"/>
+      <c r="J80" s="43"/>
       <c r="K80" s="36"/>
       <c r="L80" s="36"/>
       <c r="M80" s="37"/>
@@ -4003,7 +4021,7 @@
       <c r="G81" s="36"/>
       <c r="H81" s="37"/>
       <c r="I81" s="36"/>
-      <c r="J81" s="47"/>
+      <c r="J81" s="43"/>
       <c r="K81" s="36"/>
       <c r="L81" s="36"/>
       <c r="M81" s="37"/>
@@ -4034,7 +4052,7 @@
       <c r="G82" s="36"/>
       <c r="H82" s="37"/>
       <c r="I82" s="36"/>
-      <c r="J82" s="36"/>
+      <c r="J82" s="43"/>
       <c r="K82" s="36"/>
       <c r="L82" s="36"/>
       <c r="M82" s="37"/>
@@ -4065,7 +4083,7 @@
       <c r="G83" s="36"/>
       <c r="H83" s="37"/>
       <c r="I83" s="36"/>
-      <c r="J83" s="36"/>
+      <c r="J83" s="43"/>
       <c r="K83" s="36"/>
       <c r="L83" s="36"/>
       <c r="M83" s="37"/>
@@ -4096,7 +4114,7 @@
       <c r="G84" s="36"/>
       <c r="H84" s="37"/>
       <c r="I84" s="36"/>
-      <c r="J84" s="47"/>
+      <c r="J84" s="43"/>
       <c r="K84" s="36"/>
       <c r="L84" s="36"/>
       <c r="M84" s="37"/>
@@ -4127,7 +4145,7 @@
       <c r="G85" s="36"/>
       <c r="H85" s="37"/>
       <c r="I85" s="36"/>
-      <c r="J85" s="47"/>
+      <c r="J85" s="43"/>
       <c r="K85" s="36"/>
       <c r="L85" s="36"/>
       <c r="M85" s="37"/>
@@ -4158,7 +4176,7 @@
       <c r="G86" s="36"/>
       <c r="H86" s="37"/>
       <c r="I86" s="36"/>
-      <c r="J86" s="36"/>
+      <c r="J86" s="43"/>
       <c r="K86" s="36"/>
       <c r="L86" s="36"/>
       <c r="M86" s="37"/>
@@ -4189,7 +4207,7 @@
       <c r="G87" s="36"/>
       <c r="H87" s="37"/>
       <c r="I87" s="36"/>
-      <c r="J87" s="36"/>
+      <c r="J87" s="43"/>
       <c r="K87" s="36"/>
       <c r="L87" s="36"/>
       <c r="M87" s="37"/>
@@ -4220,7 +4238,7 @@
       <c r="G88" s="44"/>
       <c r="H88" s="37"/>
       <c r="I88" s="36"/>
-      <c r="J88" s="36"/>
+      <c r="J88" s="43"/>
       <c r="K88" s="36"/>
       <c r="L88" s="36"/>
       <c r="M88" s="37"/>
@@ -4251,7 +4269,7 @@
       <c r="G89" s="44"/>
       <c r="H89" s="37"/>
       <c r="I89" s="36"/>
-      <c r="J89" s="36"/>
+      <c r="J89" s="43"/>
       <c r="K89" s="36"/>
       <c r="L89" s="36"/>
       <c r="M89" s="37"/>
@@ -4282,7 +4300,7 @@
       <c r="G90" s="44"/>
       <c r="H90" s="37"/>
       <c r="I90" s="36"/>
-      <c r="J90" s="47"/>
+      <c r="J90" s="43"/>
       <c r="K90" s="36"/>
       <c r="L90" s="36"/>
       <c r="M90" s="37"/>
@@ -4313,7 +4331,7 @@
       <c r="G91" s="36"/>
       <c r="H91" s="37"/>
       <c r="I91" s="36"/>
-      <c r="J91" s="47"/>
+      <c r="J91" s="43"/>
       <c r="K91" s="36"/>
       <c r="L91" s="36"/>
       <c r="M91" s="37"/>
@@ -4344,7 +4362,7 @@
       <c r="G92" s="36"/>
       <c r="H92" s="37"/>
       <c r="I92" s="36"/>
-      <c r="J92" s="36"/>
+      <c r="J92" s="43"/>
       <c r="K92" s="36"/>
       <c r="L92" s="36"/>
       <c r="M92" s="37"/>
@@ -4375,7 +4393,7 @@
       <c r="G93" s="36"/>
       <c r="H93" s="37"/>
       <c r="I93" s="36"/>
-      <c r="J93" s="36"/>
+      <c r="J93" s="43"/>
       <c r="K93" s="36"/>
       <c r="L93" s="36"/>
       <c r="M93" s="37"/>
@@ -4406,7 +4424,7 @@
       <c r="G94" s="36"/>
       <c r="H94" s="37"/>
       <c r="I94" s="36"/>
-      <c r="J94" s="47"/>
+      <c r="J94" s="43"/>
       <c r="K94" s="36"/>
       <c r="L94" s="36"/>
       <c r="M94" s="37"/>
@@ -4437,7 +4455,7 @@
       <c r="G95" s="36"/>
       <c r="H95" s="37"/>
       <c r="I95" s="36"/>
-      <c r="J95" s="47"/>
+      <c r="J95" s="43"/>
       <c r="K95" s="36"/>
       <c r="L95" s="36"/>
       <c r="M95" s="37"/>
@@ -4468,7 +4486,7 @@
       <c r="G96" s="36"/>
       <c r="H96" s="37"/>
       <c r="I96" s="36"/>
-      <c r="J96" s="36"/>
+      <c r="J96" s="43"/>
       <c r="K96" s="36"/>
       <c r="L96" s="36"/>
       <c r="M96" s="37"/>
@@ -4499,7 +4517,7 @@
       <c r="G97" s="36"/>
       <c r="H97" s="37"/>
       <c r="I97" s="36"/>
-      <c r="J97" s="36"/>
+      <c r="J97" s="43"/>
       <c r="K97" s="36"/>
       <c r="L97" s="36"/>
       <c r="M97" s="37"/>
@@ -4530,7 +4548,7 @@
       <c r="G98" s="36"/>
       <c r="H98" s="37"/>
       <c r="I98" s="36"/>
-      <c r="J98" s="47"/>
+      <c r="J98" s="43"/>
       <c r="K98" s="36"/>
       <c r="L98" s="36"/>
       <c r="M98" s="37"/>
@@ -4561,7 +4579,7 @@
       <c r="G99" s="36"/>
       <c r="H99" s="37"/>
       <c r="I99" s="36"/>
-      <c r="J99" s="47"/>
+      <c r="J99" s="43"/>
       <c r="K99" s="36"/>
       <c r="L99" s="36"/>
       <c r="M99" s="37"/>
@@ -4592,7 +4610,7 @@
       <c r="G100" s="36"/>
       <c r="H100" s="37"/>
       <c r="I100" s="36"/>
-      <c r="J100" s="36"/>
+      <c r="J100" s="43"/>
       <c r="K100" s="36"/>
       <c r="L100" s="36"/>
       <c r="M100" s="37"/>
@@ -4623,7 +4641,7 @@
       <c r="G101" s="36"/>
       <c r="H101" s="37"/>
       <c r="I101" s="36"/>
-      <c r="J101" s="36"/>
+      <c r="J101" s="43"/>
       <c r="K101" s="36"/>
       <c r="L101" s="36"/>
       <c r="M101" s="37"/>
@@ -4654,7 +4672,7 @@
       <c r="G102" s="44"/>
       <c r="H102" s="37"/>
       <c r="I102" s="36"/>
-      <c r="J102" s="36"/>
+      <c r="J102" s="43"/>
       <c r="K102" s="36"/>
       <c r="L102" s="36"/>
       <c r="M102" s="37"/>
@@ -4685,7 +4703,7 @@
       <c r="G103" s="44"/>
       <c r="H103" s="37"/>
       <c r="I103" s="36"/>
-      <c r="J103" s="36"/>
+      <c r="J103" s="43"/>
       <c r="K103" s="36"/>
       <c r="L103" s="36"/>
       <c r="M103" s="37"/>
@@ -4716,7 +4734,7 @@
       <c r="G104" s="44"/>
       <c r="H104" s="37"/>
       <c r="I104" s="36"/>
-      <c r="J104" s="47"/>
+      <c r="J104" s="43"/>
       <c r="K104" s="36"/>
       <c r="L104" s="36"/>
       <c r="M104" s="37"/>
@@ -4747,7 +4765,7 @@
       <c r="G105" s="36"/>
       <c r="H105" s="37"/>
       <c r="I105" s="36"/>
-      <c r="J105" s="47"/>
+      <c r="J105" s="43"/>
       <c r="K105" s="36"/>
       <c r="L105" s="36"/>
       <c r="M105" s="37"/>
@@ -4778,7 +4796,7 @@
       <c r="G106" s="36"/>
       <c r="H106" s="37"/>
       <c r="I106" s="36"/>
-      <c r="J106" s="36"/>
+      <c r="J106" s="43"/>
       <c r="K106" s="36"/>
       <c r="L106" s="36"/>
       <c r="M106" s="37"/>
@@ -4809,7 +4827,7 @@
       <c r="G107" s="36"/>
       <c r="H107" s="37"/>
       <c r="I107" s="36"/>
-      <c r="J107" s="36"/>
+      <c r="J107" s="43"/>
       <c r="K107" s="36"/>
       <c r="L107" s="36"/>
       <c r="M107" s="37"/>
@@ -4840,7 +4858,7 @@
       <c r="G108" s="36"/>
       <c r="H108" s="37"/>
       <c r="I108" s="36"/>
-      <c r="J108" s="47"/>
+      <c r="J108" s="43"/>
       <c r="K108" s="36"/>
       <c r="L108" s="36"/>
       <c r="M108" s="37"/>
@@ -4871,7 +4889,7 @@
       <c r="G109" s="36"/>
       <c r="H109" s="37"/>
       <c r="I109" s="36"/>
-      <c r="J109" s="47"/>
+      <c r="J109" s="43"/>
       <c r="K109" s="36"/>
       <c r="L109" s="36"/>
       <c r="M109" s="37"/>
@@ -4902,7 +4920,7 @@
       <c r="G110" s="36"/>
       <c r="H110" s="37"/>
       <c r="I110" s="36"/>
-      <c r="J110" s="36"/>
+      <c r="J110" s="43"/>
       <c r="K110" s="36"/>
       <c r="L110" s="36"/>
       <c r="M110" s="37"/>
@@ -4933,7 +4951,7 @@
       <c r="G111" s="36"/>
       <c r="H111" s="37"/>
       <c r="I111" s="36"/>
-      <c r="J111" s="36"/>
+      <c r="J111" s="43"/>
       <c r="K111" s="36"/>
       <c r="L111" s="36"/>
       <c r="M111" s="37"/>
@@ -4964,7 +4982,7 @@
       <c r="G112" s="36"/>
       <c r="H112" s="37"/>
       <c r="I112" s="36"/>
-      <c r="J112" s="47"/>
+      <c r="J112" s="43"/>
       <c r="K112" s="36"/>
       <c r="L112" s="36"/>
       <c r="M112" s="37"/>
@@ -4995,7 +5013,7 @@
       <c r="G113" s="36"/>
       <c r="H113" s="37"/>
       <c r="I113" s="36"/>
-      <c r="J113" s="47"/>
+      <c r="J113" s="43"/>
       <c r="K113" s="36"/>
       <c r="L113" s="36"/>
       <c r="M113" s="37"/>
@@ -5026,7 +5044,7 @@
       <c r="G114" s="36"/>
       <c r="H114" s="37"/>
       <c r="I114" s="36"/>
-      <c r="J114" s="36"/>
+      <c r="J114" s="43"/>
       <c r="K114" s="36"/>
       <c r="L114" s="36"/>
       <c r="M114" s="37"/>
@@ -5057,7 +5075,7 @@
       <c r="G115" s="36"/>
       <c r="H115" s="37"/>
       <c r="I115" s="36"/>
-      <c r="J115" s="36"/>
+      <c r="J115" s="43"/>
       <c r="K115" s="36"/>
       <c r="L115" s="36"/>
       <c r="M115" s="37"/>
@@ -5088,7 +5106,7 @@
       <c r="G116" s="44"/>
       <c r="H116" s="37"/>
       <c r="I116" s="36"/>
-      <c r="J116" s="36"/>
+      <c r="J116" s="43"/>
       <c r="K116" s="36"/>
       <c r="L116" s="36"/>
       <c r="M116" s="37"/>
@@ -5119,7 +5137,7 @@
       <c r="G117" s="44"/>
       <c r="H117" s="37"/>
       <c r="I117" s="36"/>
-      <c r="J117" s="36"/>
+      <c r="J117" s="43"/>
       <c r="K117" s="36"/>
       <c r="L117" s="36"/>
       <c r="M117" s="37"/>
@@ -5150,7 +5168,7 @@
       <c r="G118" s="44"/>
       <c r="H118" s="37"/>
       <c r="I118" s="36"/>
-      <c r="J118" s="47"/>
+      <c r="J118" s="43"/>
       <c r="K118" s="36"/>
       <c r="L118" s="36"/>
       <c r="M118" s="37"/>
@@ -5181,7 +5199,7 @@
       <c r="G119" s="36"/>
       <c r="H119" s="37"/>
       <c r="I119" s="36"/>
-      <c r="J119" s="47"/>
+      <c r="J119" s="43"/>
       <c r="K119" s="36"/>
       <c r="L119" s="36"/>
       <c r="M119" s="37"/>
@@ -5212,7 +5230,7 @@
       <c r="G120" s="36"/>
       <c r="H120" s="37"/>
       <c r="I120" s="36"/>
-      <c r="J120" s="36"/>
+      <c r="J120" s="43"/>
       <c r="K120" s="36"/>
       <c r="L120" s="36"/>
       <c r="M120" s="37"/>
@@ -5243,7 +5261,7 @@
       <c r="G121" s="36"/>
       <c r="H121" s="37"/>
       <c r="I121" s="36"/>
-      <c r="J121" s="36"/>
+      <c r="J121" s="43"/>
       <c r="K121" s="36"/>
       <c r="L121" s="36"/>
       <c r="M121" s="37"/>
@@ -5274,7 +5292,7 @@
       <c r="G122" s="36"/>
       <c r="H122" s="37"/>
       <c r="I122" s="36"/>
-      <c r="J122" s="47"/>
+      <c r="J122" s="43"/>
       <c r="K122" s="36"/>
       <c r="L122" s="36"/>
       <c r="M122" s="37"/>
@@ -5305,7 +5323,7 @@
       <c r="G123" s="36"/>
       <c r="H123" s="37"/>
       <c r="I123" s="36"/>
-      <c r="J123" s="47"/>
+      <c r="J123" s="43"/>
       <c r="K123" s="36"/>
       <c r="L123" s="36"/>
       <c r="M123" s="37"/>
@@ -5336,7 +5354,7 @@
       <c r="G124" s="36"/>
       <c r="H124" s="37"/>
       <c r="I124" s="36"/>
-      <c r="J124" s="36"/>
+      <c r="J124" s="43"/>
       <c r="K124" s="36"/>
       <c r="L124" s="36"/>
       <c r="M124" s="37"/>
@@ -5367,7 +5385,7 @@
       <c r="G125" s="36"/>
       <c r="H125" s="37"/>
       <c r="I125" s="36"/>
-      <c r="J125" s="36"/>
+      <c r="J125" s="43"/>
       <c r="K125" s="36"/>
       <c r="L125" s="36"/>
       <c r="M125" s="37"/>
@@ -5398,7 +5416,7 @@
       <c r="G126" s="44"/>
       <c r="H126" s="37"/>
       <c r="I126" s="36"/>
-      <c r="J126" s="36"/>
+      <c r="J126" s="43"/>
       <c r="K126" s="36"/>
       <c r="L126" s="36"/>
       <c r="M126" s="37"/>
@@ -5429,7 +5447,7 @@
       <c r="G127" s="44"/>
       <c r="H127" s="37"/>
       <c r="I127" s="36"/>
-      <c r="J127" s="36"/>
+      <c r="J127" s="43"/>
       <c r="K127" s="36"/>
       <c r="L127" s="36"/>
       <c r="M127" s="37"/>
@@ -5460,7 +5478,7 @@
       <c r="G128" s="44"/>
       <c r="H128" s="37"/>
       <c r="I128" s="36"/>
-      <c r="J128" s="47"/>
+      <c r="J128" s="43"/>
       <c r="K128" s="36"/>
       <c r="L128" s="36"/>
       <c r="M128" s="37"/>
@@ -5491,7 +5509,7 @@
       <c r="G129" s="36"/>
       <c r="H129" s="37"/>
       <c r="I129" s="36"/>
-      <c r="J129" s="47"/>
+      <c r="J129" s="43"/>
       <c r="K129" s="36"/>
       <c r="L129" s="36"/>
       <c r="M129" s="37"/>
@@ -5522,7 +5540,7 @@
       <c r="G130" s="36"/>
       <c r="H130" s="37"/>
       <c r="I130" s="36"/>
-      <c r="J130" s="36"/>
+      <c r="J130" s="43"/>
       <c r="K130" s="36"/>
       <c r="L130" s="36"/>
       <c r="M130" s="37"/>
@@ -5553,7 +5571,7 @@
       <c r="G131" s="36"/>
       <c r="H131" s="37"/>
       <c r="I131" s="36"/>
-      <c r="J131" s="36"/>
+      <c r="J131" s="43"/>
       <c r="K131" s="36"/>
       <c r="L131" s="36"/>
       <c r="M131" s="37"/>
@@ -5584,7 +5602,7 @@
       <c r="G132" s="36"/>
       <c r="H132" s="37"/>
       <c r="I132" s="36"/>
-      <c r="J132" s="47"/>
+      <c r="J132" s="43"/>
       <c r="K132" s="36"/>
       <c r="L132" s="36"/>
       <c r="M132" s="37"/>
@@ -5615,7 +5633,7 @@
       <c r="G133" s="36"/>
       <c r="H133" s="37"/>
       <c r="I133" s="36"/>
-      <c r="J133" s="47"/>
+      <c r="J133" s="43"/>
       <c r="K133" s="36"/>
       <c r="L133" s="36"/>
       <c r="M133" s="37"/>
@@ -5646,7 +5664,7 @@
       <c r="G134" s="36"/>
       <c r="H134" s="37"/>
       <c r="I134" s="36"/>
-      <c r="J134" s="36"/>
+      <c r="J134" s="43"/>
       <c r="K134" s="36"/>
       <c r="L134" s="36"/>
       <c r="M134" s="37"/>
@@ -5677,7 +5695,7 @@
       <c r="G135" s="36"/>
       <c r="H135" s="37"/>
       <c r="I135" s="36"/>
-      <c r="J135" s="36"/>
+      <c r="J135" s="43"/>
       <c r="K135" s="36"/>
       <c r="L135" s="36"/>
       <c r="M135" s="37"/>
@@ -5708,7 +5726,7 @@
       <c r="G136" s="36"/>
       <c r="H136" s="37"/>
       <c r="I136" s="36"/>
-      <c r="J136" s="47"/>
+      <c r="J136" s="43"/>
       <c r="K136" s="36"/>
       <c r="L136" s="36"/>
       <c r="M136" s="37"/>
@@ -5739,7 +5757,7 @@
       <c r="G137" s="36"/>
       <c r="H137" s="37"/>
       <c r="I137" s="36"/>
-      <c r="J137" s="47"/>
+      <c r="J137" s="43"/>
       <c r="K137" s="36"/>
       <c r="L137" s="36"/>
       <c r="M137" s="37"/>
@@ -5770,7 +5788,7 @@
       <c r="G138" s="36"/>
       <c r="H138" s="37"/>
       <c r="I138" s="36"/>
-      <c r="J138" s="36"/>
+      <c r="J138" s="43"/>
       <c r="K138" s="36"/>
       <c r="L138" s="36"/>
       <c r="M138" s="37"/>
@@ -5801,7 +5819,7 @@
       <c r="G139" s="36"/>
       <c r="H139" s="37"/>
       <c r="I139" s="36"/>
-      <c r="J139" s="36"/>
+      <c r="J139" s="43"/>
       <c r="K139" s="36"/>
       <c r="L139" s="36"/>
       <c r="M139" s="37"/>
@@ -5832,7 +5850,7 @@
       <c r="G140" s="44"/>
       <c r="H140" s="37"/>
       <c r="I140" s="36"/>
-      <c r="J140" s="36"/>
+      <c r="J140" s="43"/>
       <c r="K140" s="36"/>
       <c r="L140" s="36"/>
       <c r="M140" s="37"/>
@@ -5863,7 +5881,7 @@
       <c r="G141" s="44"/>
       <c r="H141" s="37"/>
       <c r="I141" s="36"/>
-      <c r="J141" s="36"/>
+      <c r="J141" s="43"/>
       <c r="K141" s="36"/>
       <c r="L141" s="36"/>
       <c r="M141" s="37"/>
@@ -5894,7 +5912,7 @@
       <c r="G142" s="44"/>
       <c r="H142" s="37"/>
       <c r="I142" s="36"/>
-      <c r="J142" s="47"/>
+      <c r="J142" s="43"/>
       <c r="K142" s="36"/>
       <c r="L142" s="36"/>
       <c r="M142" s="37"/>
@@ -5925,7 +5943,7 @@
       <c r="G143" s="36"/>
       <c r="H143" s="37"/>
       <c r="I143" s="36"/>
-      <c r="J143" s="47"/>
+      <c r="J143" s="43"/>
       <c r="K143" s="36"/>
       <c r="L143" s="36"/>
       <c r="M143" s="37"/>
@@ -5956,7 +5974,7 @@
       <c r="G144" s="36"/>
       <c r="H144" s="37"/>
       <c r="I144" s="36"/>
-      <c r="J144" s="36"/>
+      <c r="J144" s="43"/>
       <c r="K144" s="36"/>
       <c r="L144" s="36"/>
       <c r="M144" s="37"/>
@@ -5987,7 +6005,7 @@
       <c r="G145" s="36"/>
       <c r="H145" s="37"/>
       <c r="I145" s="36"/>
-      <c r="J145" s="36"/>
+      <c r="J145" s="43"/>
       <c r="K145" s="36"/>
       <c r="L145" s="36"/>
       <c r="M145" s="37"/>
@@ -6018,7 +6036,7 @@
       <c r="G146" s="36"/>
       <c r="H146" s="37"/>
       <c r="I146" s="36"/>
-      <c r="J146" s="47"/>
+      <c r="J146" s="43"/>
       <c r="K146" s="36"/>
       <c r="L146" s="36"/>
       <c r="M146" s="37"/>
@@ -6049,7 +6067,7 @@
       <c r="G147" s="36"/>
       <c r="H147" s="37"/>
       <c r="I147" s="36"/>
-      <c r="J147" s="47"/>
+      <c r="J147" s="43"/>
       <c r="K147" s="36"/>
       <c r="L147" s="36"/>
       <c r="M147" s="37"/>
@@ -6080,7 +6098,7 @@
       <c r="G148" s="36"/>
       <c r="H148" s="37"/>
       <c r="I148" s="36"/>
-      <c r="J148" s="36"/>
+      <c r="J148" s="43"/>
       <c r="K148" s="36"/>
       <c r="L148" s="36"/>
       <c r="M148" s="37"/>
@@ -6111,7 +6129,7 @@
       <c r="G149" s="36"/>
       <c r="H149" s="37"/>
       <c r="I149" s="36"/>
-      <c r="J149" s="36"/>
+      <c r="J149" s="43"/>
       <c r="K149" s="36"/>
       <c r="L149" s="36"/>
       <c r="M149" s="37"/>
@@ -6133,25 +6151,25 @@
       <c r="Z149" s="45"/>
     </row>
     <row r="150" spans="1:26" ht="25.5" customHeight="1">
-      <c r="A150" s="94" t="s">
+      <c r="A150" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="B150" s="94"/>
-      <c r="C150" s="94"/>
-      <c r="D150" s="94"/>
-      <c r="E150" s="94"/>
-      <c r="F150" s="94"/>
-      <c r="G150" s="94"/>
-      <c r="H150" s="94"/>
-      <c r="I150" s="94"/>
-      <c r="J150" s="94"/>
-      <c r="K150" s="94"/>
-      <c r="L150" s="94"/>
-      <c r="M150" s="94"/>
-      <c r="N150" s="94"/>
-      <c r="O150" s="94"/>
-      <c r="P150" s="94"/>
-      <c r="Q150" s="94"/>
+      <c r="B150" s="77"/>
+      <c r="C150" s="77"/>
+      <c r="D150" s="77"/>
+      <c r="E150" s="77"/>
+      <c r="F150" s="77"/>
+      <c r="G150" s="77"/>
+      <c r="H150" s="77"/>
+      <c r="I150" s="77"/>
+      <c r="J150" s="77"/>
+      <c r="K150" s="77"/>
+      <c r="L150" s="77"/>
+      <c r="M150" s="77"/>
+      <c r="N150" s="77"/>
+      <c r="O150" s="77"/>
+      <c r="P150" s="77"/>
+      <c r="Q150" s="77"/>
       <c r="R150" s="50"/>
       <c r="S150" s="51"/>
       <c r="T150" s="51"/>
@@ -6175,7 +6193,7 @@
       <c r="G151" s="58"/>
       <c r="H151" s="59"/>
       <c r="I151" s="58"/>
-      <c r="J151" s="58"/>
+      <c r="J151" s="105"/>
       <c r="K151" s="58"/>
       <c r="L151" s="58"/>
       <c r="M151" s="58"/>
@@ -6200,18 +6218,18 @@
       </c>
       <c r="C152" s="64"/>
       <c r="D152" s="65"/>
-      <c r="E152" s="95">
+      <c r="E152" s="78">
         <f>+E9+E10</f>
         <v>1899002428.4285715</v>
       </c>
-      <c r="F152" s="95"/>
+      <c r="F152" s="78"/>
       <c r="G152" s="64"/>
       <c r="H152" s="66">
         <f>+H9+H10</f>
         <v>0</v>
       </c>
       <c r="I152" s="7"/>
-      <c r="J152" s="7"/>
+      <c r="J152" s="106"/>
       <c r="K152" s="7"/>
       <c r="L152" s="7"/>
       <c r="M152" s="7" t="s">
@@ -6227,6 +6245,31 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="Q3:Z3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="Q4:Z4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="Q5:Z5"/>
+    <mergeCell ref="A6:Z6"/>
+    <mergeCell ref="A7:Z7"/>
+    <mergeCell ref="C8:Z8"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
     <mergeCell ref="Y12:Y13"/>
     <mergeCell ref="Z12:Z13"/>
     <mergeCell ref="A150:Q150"/>
@@ -6243,31 +6286,6 @@
     <mergeCell ref="P12:P13"/>
     <mergeCell ref="Q12:Q13"/>
     <mergeCell ref="R12:R13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="Q3:Z3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="Q4:Z4"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="Q5:Z5"/>
-    <mergeCell ref="A6:Z6"/>
-    <mergeCell ref="A7:Z7"/>
-    <mergeCell ref="C8:Z8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" xr:uid="{D88860E5-26A2-400E-9CD6-A0A7F92B8419}"/>

</xml_diff>